<commit_message>
Code formatting and design decisions update
</commit_message>
<xml_diff>
--- a/background_docs/Video/Design decisions tracking.xlsx
+++ b/background_docs/Video/Design decisions tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\COMP0022_Coursework\background_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\freebay\COMP0022_Coursework\background_docs\Video\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D97A3D7-DF03-483A-97B7-D8786BF05E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381A6CC2-2C38-421B-8A90-B30DD1F42F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>Requirement 1</t>
   </si>
@@ -257,6 +256,57 @@
       <t xml:space="preserve">
 NB to you guys: I will also discuss this in the report, but should still be voiced over in some form in the video too</t>
     </r>
+  </si>
+  <si>
+    <t>The bid form is only available to buyers who are logged in, and only before the auction end date.</t>
+  </si>
+  <si>
+    <t>This is to prevent sellers and users who are not logged in from making a bid.</t>
+  </si>
+  <si>
+    <t>When a bid is placed, we check if the auction end date is in the past.</t>
+  </si>
+  <si>
+    <t>This it to prevent users from loading the listing page, waiting for the auction to end, and then submitting a bid.</t>
+  </si>
+  <si>
+    <t>Number of watchers is shown in the listing page, and updated live when the user adds or removes the listing from their watchlist</t>
+  </si>
+  <si>
+    <t>When a bid is placed on an auction that the buyer doesn't have on their wathclist, they are prompted to add to watchlist</t>
+  </si>
+  <si>
+    <t>When a bid is placed, all buyers who have the auction on their watchlist receive an email notification. Only the previous highest bidder is notified that they were outbid.</t>
+  </si>
+  <si>
+    <t>Summary information is shown for each auction. This varies depending on whether the auction has ended or not.</t>
+  </si>
+  <si>
+    <t>Bid history (bid amount, bid date, and bid username) for each auction is visible to all users.</t>
+  </si>
+  <si>
+    <t>Auctions that have ended have more limited information - they exlude starting price and minimum increment, but include final price.</t>
+  </si>
+  <si>
+    <t>All users are able to see bid history, including those who are not logged in.</t>
+  </si>
+  <si>
+    <t>When a bid is placed, we verify the bid amount and format - only numbers with up to 2 decimal points allowed, and only numbers &gt;= minimum bid are allowed (min. bid determined by current price and min. increment)</t>
+  </si>
+  <si>
+    <t>The bid input is quite crucial to the whole website, so we validate it both on the front end through the bid form, and in the back end through a SQL function.</t>
+  </si>
+  <si>
+    <t>Buyers have a My Bids tab, where they can see, filter and sort all auctions they've bid on, and all individual bids. They also see what the current highest bid is, as well as who's winning the auction.</t>
+  </si>
+  <si>
+    <t>Buyers have a My Watchlist tab, where they can see all their watched auctions, filter and sort them, as well as remove auctions from watchlist. They also see the current highest bid and bidder.</t>
+  </si>
+  <si>
+    <t>This page has a lot of overlap with the My Bids page, but the key difference is that buyers can use this to track auctions before deciding whether to bid or not.</t>
+  </si>
+  <si>
+    <t>When an auction ends, both buyers and sellers can see the outcome through the My Bids/My Watchlist and My Listings pages respectively. In addition, sellers receive an email notifying them of their auction's outcome, and winning buyers will also receive an email notification.</t>
   </si>
 </sst>
 </file>
@@ -652,21 +702,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C03CD6-D467-46A7-A458-3DEB0FCCC033}">
   <dimension ref="A2:C41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="73.26953125" customWidth="1"/>
-    <col min="3" max="3" width="85.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -674,7 +724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
@@ -682,7 +732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="7" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
@@ -690,7 +740,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
@@ -698,7 +748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="7" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
@@ -706,7 +756,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
@@ -714,7 +764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -722,7 +772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -730,7 +780,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
@@ -738,7 +788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="5" t="s">
         <v>15</v>
@@ -747,7 +797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
@@ -755,7 +805,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
@@ -763,7 +813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>18</v>
       </c>
@@ -771,7 +821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:3" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
@@ -779,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:3" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>28</v>
       </c>
@@ -787,7 +837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:3" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
@@ -795,7 +845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:3" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
@@ -803,87 +853,87 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
     </row>
@@ -899,19 +949,19 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="68.7265625" customWidth="1"/>
-    <col min="3" max="3" width="85.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -919,132 +969,132 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
@@ -1060,19 +1110,19 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="68.7265625" customWidth="1"/>
-    <col min="3" max="3" width="85.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1080,132 +1130,132 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
@@ -1219,21 +1269,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF41A9BB-0F1C-4A77-81C6-768EF23F0EC9}">
   <dimension ref="A2:C27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="68.7265625" customWidth="1"/>
-    <col min="3" max="3" width="85.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1241,82 +1293,106 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="5"/>
+    <row r="11" spans="1:3" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>43</v>
       </c>
@@ -1324,7 +1400,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:3" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
@@ -1332,7 +1408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:3" s="2" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" s="2" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>47</v>
       </c>
@@ -1340,7 +1416,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="2:3" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>38</v>
       </c>
@@ -1348,7 +1424,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>50</v>
       </c>
@@ -1366,21 +1442,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94C738F-1C06-49F2-8FD4-3A23FFBAA1BD}">
   <dimension ref="A2:C36"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="68.7265625" customWidth="1"/>
-    <col min="3" max="3" width="85.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1388,132 +1466,142 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
+    <row r="5" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5"/>
+    <row r="6" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
+    <row r="7" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
@@ -1529,19 +1617,19 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="68.7265625" customWidth="1"/>
-    <col min="3" max="3" width="85.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" customWidth="1"/>
+    <col min="3" max="3" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1549,7 +1637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>35</v>
       </c>
@@ -1557,7 +1645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" ht="143.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="2" customFormat="1" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>48</v>
       </c>
@@ -1565,7 +1653,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
@@ -1573,7 +1661,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>40</v>
@@ -1582,115 +1670,115 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>

</xml_diff>

<commit_message>
Fixed issue in check_auction_end
</commit_message>
<xml_diff>
--- a/background_docs/Video/Design decisions tracking.xlsx
+++ b/background_docs/Video/Design decisions tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\freebay\COMP0022_Coursework\background_docs\Video\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381A6CC2-2C38-421B-8A90-B30DD1F42F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94851DF-D1C7-4E9C-91B9-E6BA7001EA9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
   <si>
     <t>Requirement 1</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>When an auction ends, both buyers and sellers can see the outcome through the My Bids/My Watchlist and My Listings pages respectively. In addition, sellers receive an email notifying them of their auction's outcome, and winning buyers will also receive an email notification.</t>
+  </si>
+  <si>
+    <t>If a finished auction is on a buyer's watchlist, they only have the option to remove it from watchlist.</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -418,6 +421,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1269,9 +1275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF41A9BB-0F1C-4A77-81C6-768EF23F0EC9}">
   <dimension ref="A2:C27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1294,7 +1298,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1302,7 +1306,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1310,7 +1314,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1319,7 +1323,7 @@
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1327,7 +1331,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1335,13 +1339,13 @@
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="9" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C11" s="5"/>
@@ -1443,7 +1447,7 @@
   <dimension ref="A2:C36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,34 +1471,36 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+    <row r="9" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>